<commit_message>
closes #11, #2, working on #7
</commit_message>
<xml_diff>
--- a/src/data/copy.xlsx
+++ b/src/data/copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoyoyo/src/china-pathfinder/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB3B29D-F595-7F4F-B5F1-118595C4DB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165F7E67-0186-4B45-9115-AE692F142D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45200" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{2CA29B29-CA57-8848-BDC1-AB78C1F4C6BF}"/>
+    <workbookView xWindow="7260" yWindow="560" windowWidth="33600" windowHeight="20540" xr2:uid="{2CA29B29-CA57-8848-BDC1-AB78C1F4C6BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -60,24 +60,15 @@
     <t>Portfolio Investment Openness</t>
   </si>
   <si>
-    <t>Portfolio investment openness refers to limited controls on two-way cross-border investment into equities, debt, and other financial instruments. Portfolio investment openness is a key ingredient for financial market efficiency and market-driven exchange rate adjustments in open market economies.</t>
-  </si>
-  <si>
     <t>Direct Investment Openness</t>
   </si>
   <si>
     <t>FDI</t>
   </si>
   <si>
-    <t>Foreign Direct Investment (FDI) openness refers to fair, non-discriminatory access for foreign firms to domestic markets and freedom for domestic companies to invest abroad without restrictions or political mandates. FDI openness is a key feature of open market economies to encourage competitive markets and facilitate the global division of labor based on comparative advantages.</t>
-  </si>
-  <si>
     <t>Beijing has gradually opened to inbound FDI by moving from an approval-based system to a negative list-based system and reducing restricted sectors for foreign investment, but foreign and domestic investments are not treated equally in many sectors of the economy. Chinese companies continue to face major restrictions and political interventions for overseas investments, and those restrictions have increased since 2016.</t>
   </si>
   <si>
-    <t>Market economies rely on innovation to drive competition, increase productivity, and create wealth. Innovation system designs vary across countries, but market economies generally employ systems that rely on government funding for basic research but emphasize private sector investment; encourage the commercial application of knowledge through the strong protection of intellectual property rights, and encourage collaboration with and participation of foreign firms and researchers.</t>
-  </si>
-  <si>
     <t>Innovation</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>While China has a storied history of invention and produces renowned innovators, its innovation system has diverged from advanced market economies in important ways throughout the modern era. Even as China is reaching middle income status, its innovation system continues to feature (1) compulsive technology policies; (2) preponderance of state intervention and industrial policies across a wide range of technologies; (3) strong biases in support of domestic firms and researchers; and (4) lax credit terms at volume in support of innovation. Under President Xi’s leadership, China has doubled down on these policies in recent years. This has led to global concerns about Chinese innovation mercantilism and possible negative impacts on global innovative capacity in the long run.</t>
   </si>
   <si>
-    <t xml:space="preserve">Market economies rely on a pro-competitive environment where firms face low entry/exit barriers, market power abuses are disciplined, consumer interests are prioritized, government participation in the marketplace is limited and justified by clear pro-competitive principles. </t>
-  </si>
-  <si>
     <t>Market Competition</t>
   </si>
   <si>
@@ -105,9 +93,6 @@
     <t>Financial System Development</t>
   </si>
   <si>
-    <t>Open market economies rely on modern financial systems for the efficient pricing of risk and allocation of capital. Key pillars of modern financial systems are market-driven credit pricing, availability of a broad range of financial instruments, the absence of distortive administrative controls on credit price and quantity, and access for foreign firms to financial services and foreign exchange markets.</t>
-  </si>
-  <si>
     <t>China’s financial system is dominated by state-related banks and political considerations. This promoted faster growth in the past but imposes a heavy toll on efficiency, structural adjustment and market allocation of capital as the nation reaches higher income levels. Reliance on this system for growth and stability stymies reforms, capital market deepening, non-bank financial institution growth, and openness to foreign competition. Market-determined interest rates – fundamental to market economies – are missing, causing the system – and risks associated with it -- to balloon beyond other economies. This is increasingly seen abroad as distorting fair trade and competition, thus justifying anti-subsidies policies toward China.  By trying too hard to prevent financial stress, the state has created it: the consequences of transitioning from the status quo are increasingly unpalatable to leaders.</t>
   </si>
   <si>
@@ -115,13 +100,31 @@
   </si>
   <si>
     <t>China has historically tightly controlled portfolio investment flows to maintain control over its exchange rate and domestic interest rates. In the past three years Beijing has accelerated reforms to gradually reduce restrictions on portfolio flows. It scrapped its long-standing inbound quota system (QFII) and established “connect” schemes for foreigners to access stock and bond markets within pre-defined quotas. It has also made regulatory changes to facilitate the inclusion of onshore securities in major global indices. However, outbound flows remain tightly restricted and state-driven, and foreign investors lack sufficient hedging tools in onshore markets.</t>
+  </si>
+  <si>
+    <t>quantifies the prominence of market-driven credit pricing, the availability of financial instruments, and the absence of distortive controls on debt.</t>
+  </si>
+  <si>
+    <t>quantifies economic dynamism by assessing the entry and exit barriers firms face, government response to market power abuses, and government participation in the marketplace.</t>
+  </si>
+  <si>
+    <t>quantifies the prevalence of a market-based innovation system by analyzing the levels of public and private sector investment, the protection of intellectual property rights, and collaboration with foreign firms.</t>
+  </si>
+  <si>
+    <t>quantifies an economy’s trade restrictiveness through measures such as tariff rates, non-tariff barriers, and the overall cross-border flow of goods and services.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantifies the level of freedom a country’s domestic companies have to invest abroad without restrictions or political mandates, and access for foreign firms to invest in its domestic markets. </t>
+  </si>
+  <si>
+    <t>quantifies a country’s controls on cross-border investment through measures of equities, bonds, debt, foreign exchange, and other financial instruments.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,6 +138,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,10 +168,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +487,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,86 +508,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix selected circle z-index bug
</commit_message>
<xml_diff>
--- a/src/data/copy.xlsx
+++ b/src/data/copy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickharb/code/2021/china-pathfinder/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E274664-C0AB-DA4F-B25C-F08C588C21D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235899B7-E0F2-434F-B118-936B8B35C0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Eget commodo a amet, maecenas imperdiet.</t>
   </si>
   <si>
-    <t>Depth and stability of financial market; minimal distortions on credit pricing and quantity; foreign firms able to access financial services and foreign exchange markets.</t>
-  </si>
-  <si>
     <t>An environment where firms face low entry/exit barriers, market power abuses are disciplined, and distortive interventions are minimized.</t>
   </si>
   <si>
@@ -452,6 +449,9 @@
   </si>
   <si>
     <t>Patent Families</t>
+  </si>
+  <si>
+    <t>A system that efficiently prices credit, allocates capital based on market signals, and provides foreign firms with access to financial services.</t>
   </si>
 </sst>
 </file>
@@ -740,7 +740,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D27" sqref="A1:I38"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -765,10 +765,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
@@ -796,7 +796,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>47</v>
@@ -821,7 +821,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>44</v>
@@ -846,7 +846,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>46</v>
@@ -871,7 +871,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>16</v>
@@ -896,7 +896,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>45</v>
@@ -921,7 +921,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>48</v>
@@ -944,10 +944,10 @@
         <v>75</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>22</v>
@@ -967,10 +967,10 @@
         <v>76</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>23</v>
@@ -990,10 +990,10 @@
         <v>77</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>24</v>
@@ -1013,10 +1013,10 @@
         <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>25</v>
@@ -1036,10 +1036,10 @@
         <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>26</v>
@@ -1059,10 +1059,10 @@
         <v>69</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>27</v>
@@ -1082,10 +1082,10 @@
         <v>70</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>28</v>
@@ -1105,10 +1105,10 @@
         <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>29</v>
@@ -1128,10 +1128,10 @@
         <v>72</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>42</v>
@@ -1151,10 +1151,10 @@
         <v>73</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>42</v>
@@ -1174,10 +1174,10 @@
         <v>65</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>30</v>
@@ -1197,10 +1197,10 @@
         <v>66</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>31</v>
@@ -1220,10 +1220,10 @@
         <v>67</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>42</v>
@@ -1243,10 +1243,10 @@
         <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>42</v>
@@ -1266,10 +1266,10 @@
         <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>42</v>
@@ -1289,10 +1289,10 @@
         <v>60</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>34</v>
@@ -1312,10 +1312,10 @@
         <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>42</v>
@@ -1335,10 +1335,10 @@
         <v>62</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>42</v>
@@ -1358,10 +1358,10 @@
         <v>63</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>42</v>
@@ -1381,10 +1381,10 @@
         <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>42</v>
@@ -1404,10 +1404,10 @@
         <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>42</v>
@@ -1427,10 +1427,10 @@
         <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>36</v>
@@ -1450,10 +1450,10 @@
         <v>56</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>37</v>
@@ -1494,10 +1494,10 @@
         <v>59</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>42</v>
@@ -1517,10 +1517,10 @@
         <v>50</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>124</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>38</v>
@@ -1540,10 +1540,10 @@
         <v>39</v>
       </c>
       <c r="D34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>40</v>
@@ -1563,10 +1563,10 @@
         <v>51</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>42</v>
@@ -1586,10 +1586,10 @@
         <v>52</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>42</v>
@@ -1609,7 +1609,7 @@
         <v>53</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="4" t="s">
@@ -1630,10 +1630,10 @@
         <v>54</v>
       </c>
       <c r="D38" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>42</v>

</xml_diff>